<commit_message>
Petite modif du planning
</commit_message>
<xml_diff>
--- a/planning/Planification.xlsx
+++ b/planning/Planification.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADRIAN.BMGRT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\var\www\html\ATProgrammationSmartphone\2eme_Semestre\GameAdvice\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E466888-6ACD-460C-A91F-D39A93FFBF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6AA923-16EF-47C2-B95C-341CBD239A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-100C]d\.\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-100C]d\.\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -847,7 +847,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -919,18 +918,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1014,8 +1001,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1117,6 +1102,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,7 +1400,7 @@
   <dimension ref="C3:AA28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,187 +1415,187 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="64"/>
+      <c r="D3" s="59"/>
     </row>
     <row r="4" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="60"/>
     </row>
     <row r="5" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="66"/>
+      <c r="D5" s="61"/>
     </row>
     <row r="6" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="67"/>
+      <c r="D6" s="62"/>
     </row>
     <row r="7" spans="3:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="123"/>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
+      <c r="Y7" s="123"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
     <row r="8" spans="3:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="1"/>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="124">
         <v>44588</v>
       </c>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48">
+      <c r="G8" s="125"/>
+      <c r="H8" s="126">
         <v>44595</v>
       </c>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48">
+      <c r="I8" s="125"/>
+      <c r="J8" s="126">
         <v>44602</v>
       </c>
-      <c r="K8" s="47"/>
-      <c r="L8" s="48">
+      <c r="K8" s="125"/>
+      <c r="L8" s="126">
         <v>44616</v>
       </c>
-      <c r="M8" s="49"/>
-      <c r="N8" s="46">
+      <c r="M8" s="127"/>
+      <c r="N8" s="124">
         <v>44623</v>
       </c>
-      <c r="O8" s="47"/>
-      <c r="P8" s="48">
+      <c r="O8" s="125"/>
+      <c r="P8" s="126">
         <v>44630</v>
       </c>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="48">
+      <c r="Q8" s="125"/>
+      <c r="R8" s="126">
         <v>44637</v>
       </c>
-      <c r="S8" s="49"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
+      <c r="S8" s="127"/>
+      <c r="T8" s="123"/>
+      <c r="U8" s="123"/>
+      <c r="V8" s="123"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="123"/>
+      <c r="Y8" s="123"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
     <row r="9" spans="3:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="25"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="24"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
     <row r="10" spans="3:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="39"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="38"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="41"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="40"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
     <row r="11" spans="3:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="29"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="33"/>
+      <c r="S11" s="32"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
     <row r="12" spans="3:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="63"/>
-      <c r="G12" s="29"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
       <c r="R12" s="16"/>
-      <c r="S12" s="33"/>
+      <c r="S12" s="32"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
     <row r="13" spans="3:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
-      <c r="E13" s="61" t="s">
+      <c r="E13" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="69"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="64"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="7"/>
@@ -1613,11 +1613,11 @@
     </row>
     <row r="14" spans="3:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
-      <c r="E14" s="61" t="s">
+      <c r="E14" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="70"/>
-      <c r="G14" s="93"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="86"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
@@ -1635,33 +1635,33 @@
     </row>
     <row r="15" spans="3:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
       <c r="R15" s="16"/>
-      <c r="S15" s="33"/>
+      <c r="S15" s="32"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
     <row r="16" spans="3:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
-      <c r="E16" s="60" t="s">
+      <c r="E16" s="55" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="66"/>
+      <c r="G16" s="61"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="7"/>
@@ -1679,15 +1679,15 @@
     </row>
     <row r="17" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="55" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="92"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="85"/>
       <c r="L17" s="7"/>
       <c r="M17" s="9"/>
       <c r="N17" s="8"/>
@@ -1701,11 +1701,11 @@
     </row>
     <row r="18" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="55" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="5"/>
-      <c r="G18" s="67"/>
+      <c r="G18" s="62"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="7"/>
@@ -1723,21 +1723,21 @@
     </row>
     <row r="19" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="74"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="73"/>
-      <c r="Q19" s="73"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="68"/>
+      <c r="P19" s="68"/>
+      <c r="Q19" s="68"/>
       <c r="R19" s="15"/>
       <c r="S19" s="12"/>
       <c r="Z19" s="1"/>
@@ -1745,56 +1745,56 @@
     </row>
     <row r="20" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="55" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="81"/>
-      <c r="Q20" s="55"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="76"/>
+      <c r="Q20" s="50"/>
       <c r="R20" s="7"/>
-      <c r="S20" s="30"/>
+      <c r="S20" s="29"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
     <row r="21" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
-      <c r="E21" s="60" t="s">
+      <c r="E21" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="76"/>
-      <c r="N21" s="82"/>
-      <c r="O21" s="83"/>
-      <c r="P21" s="84"/>
-      <c r="Q21" s="76"/>
-      <c r="R21" s="31"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="78"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="30"/>
       <c r="S21" s="17"/>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
     <row r="22" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="55" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="32"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="6"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
@@ -1802,8 +1802,8 @@
       <c r="M22" s="6"/>
       <c r="N22" s="13"/>
       <c r="O22" s="14"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="77"/>
+      <c r="P22" s="70"/>
+      <c r="Q22" s="72"/>
       <c r="R22" s="15"/>
       <c r="S22" s="12"/>
       <c r="Z22" s="1"/>
@@ -1811,29 +1811,29 @@
     </row>
     <row r="23" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="90"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="55"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
       <c r="R23" s="16"/>
-      <c r="S23" s="33"/>
+      <c r="S23" s="32"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
     <row r="24" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="55" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="5"/>
@@ -1844,78 +1844,78 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="6"/>
-      <c r="N24" s="27"/>
+      <c r="N24" s="26"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
-      <c r="Q24" s="94"/>
+      <c r="Q24" s="87"/>
       <c r="R24" s="7"/>
-      <c r="S24" s="59"/>
+      <c r="S24" s="54"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
     <row r="25" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
       <c r="R25" s="16"/>
-      <c r="S25" s="33"/>
+      <c r="S25" s="32"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
     <row r="26" spans="4:27" ht="21" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
-      <c r="E26" s="95" t="s">
+      <c r="E26" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="96"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="97"/>
-      <c r="I26" s="97"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
-      <c r="M26" s="97"/>
-      <c r="N26" s="69"/>
-      <c r="O26" s="97"/>
-      <c r="P26" s="101"/>
-      <c r="Q26" s="101"/>
-      <c r="R26" s="99"/>
-      <c r="S26" s="100"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="91"/>
+      <c r="K26" s="91"/>
+      <c r="L26" s="91"/>
+      <c r="M26" s="90"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="90"/>
+      <c r="P26" s="94"/>
+      <c r="Q26" s="94"/>
+      <c r="R26" s="92"/>
+      <c r="S26" s="93"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
     <row r="27" spans="4:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
-      <c r="E27" s="68" t="s">
+      <c r="E27" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="85"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="89"/>
-      <c r="O27" s="87"/>
-      <c r="P27" s="87"/>
-      <c r="Q27" s="87"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="35"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="129"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="82"/>
+      <c r="O27" s="80"/>
+      <c r="P27" s="80"/>
+      <c r="Q27" s="80"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="34"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
@@ -1979,446 +1979,446 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="64"/>
+      <c r="C3" s="59"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="65"/>
+      <c r="C4" s="60"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="66"/>
+      <c r="C5" s="61"/>
     </row>
     <row r="6" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="62"/>
     </row>
     <row r="7" spans="2:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
     </row>
     <row r="8" spans="2:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="124">
         <v>44588</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="48">
+      <c r="F8" s="125"/>
+      <c r="G8" s="126">
         <v>44595</v>
       </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="48">
+      <c r="H8" s="125"/>
+      <c r="I8" s="126">
         <v>44602</v>
       </c>
-      <c r="J8" s="47"/>
-      <c r="K8" s="48">
+      <c r="J8" s="125"/>
+      <c r="K8" s="126">
         <v>44616</v>
       </c>
-      <c r="L8" s="49"/>
-      <c r="M8" s="46">
+      <c r="L8" s="127"/>
+      <c r="M8" s="124">
         <v>44623</v>
       </c>
-      <c r="N8" s="47"/>
-      <c r="O8" s="48">
+      <c r="N8" s="125"/>
+      <c r="O8" s="126">
         <v>44630</v>
       </c>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="48">
+      <c r="P8" s="125"/>
+      <c r="Q8" s="126">
         <v>44637</v>
       </c>
-      <c r="R8" s="49"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54"/>
+      <c r="R8" s="127"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
     </row>
     <row r="9" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54"/>
-      <c r="V9" s="54"/>
-      <c r="W9" s="54"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
     </row>
     <row r="10" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="39"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="38"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="41"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="40"/>
     </row>
     <row r="11" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="128"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="79"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="78"/>
-      <c r="R11" s="102"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="95"/>
     </row>
     <row r="12" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="103"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="102"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="95"/>
     </row>
     <row r="13" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
-      <c r="D13" s="61" t="s">
+      <c r="D13" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="129"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="80"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="107"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="99"/>
+      <c r="R13" s="100"/>
     </row>
     <row r="14" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="70"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="105"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="80"/>
-      <c r="P14" s="80"/>
-      <c r="Q14" s="106"/>
-      <c r="R14" s="107"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="75"/>
+      <c r="P14" s="75"/>
+      <c r="Q14" s="99"/>
+      <c r="R14" s="100"/>
     </row>
     <row r="15" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="108"/>
-      <c r="F15" s="127"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="102"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="95"/>
     </row>
     <row r="16" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="102"/>
-      <c r="S16" s="54"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="73"/>
+      <c r="R16" s="95"/>
+      <c r="S16" s="49"/>
     </row>
     <row r="17" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="78"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="78"/>
-      <c r="R17" s="102"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="73"/>
+      <c r="R17" s="95"/>
     </row>
     <row r="18" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="110"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="78"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="79"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="78"/>
-      <c r="R18" s="102"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="73"/>
+      <c r="R18" s="95"/>
     </row>
     <row r="19" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="112"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="111"/>
-      <c r="M19" s="113"/>
-      <c r="N19" s="111"/>
-      <c r="O19" s="111"/>
-      <c r="P19" s="111"/>
-      <c r="Q19" s="106"/>
-      <c r="R19" s="107"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="105"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="105"/>
+      <c r="L19" s="104"/>
+      <c r="M19" s="106"/>
+      <c r="N19" s="104"/>
+      <c r="O19" s="104"/>
+      <c r="P19" s="104"/>
+      <c r="Q19" s="99"/>
+      <c r="R19" s="100"/>
     </row>
     <row r="20" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="79"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="80"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="78"/>
-      <c r="R20" s="102"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="73"/>
+      <c r="R20" s="95"/>
     </row>
     <row r="21" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="114"/>
-      <c r="O21" s="115"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="102"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="107"/>
+      <c r="O21" s="108"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="95"/>
     </row>
     <row r="22" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="80"/>
-      <c r="Q22" s="106"/>
-      <c r="R22" s="107"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="98"/>
+      <c r="N22" s="75"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="99"/>
+      <c r="R22" s="100"/>
     </row>
     <row r="23" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-      <c r="D23" s="61" t="s">
+      <c r="D23" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="116"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="102"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="73"/>
+      <c r="R23" s="95"/>
     </row>
     <row r="24" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="117"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="110"/>
     </row>
     <row r="25" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="78"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="102"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="73"/>
+      <c r="R25" s="95"/>
     </row>
     <row r="26" spans="3:23" ht="21" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
-      <c r="D26" s="95" t="s">
+      <c r="D26" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="118"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="101"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="119"/>
-      <c r="J26" s="119"/>
-      <c r="K26" s="119"/>
-      <c r="L26" s="101"/>
-      <c r="M26" s="104"/>
-      <c r="N26" s="101"/>
-      <c r="O26" s="101"/>
-      <c r="P26" s="101"/>
-      <c r="Q26" s="119"/>
-      <c r="R26" s="120"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="94"/>
+      <c r="H26" s="94"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
+      <c r="K26" s="112"/>
+      <c r="L26" s="94"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="94"/>
+      <c r="O26" s="94"/>
+      <c r="P26" s="94"/>
+      <c r="Q26" s="112"/>
+      <c r="R26" s="113"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -2427,33 +2427,33 @@
     </row>
     <row r="27" spans="3:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
-      <c r="D27" s="68" t="s">
+      <c r="D27" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="121"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="123"/>
-      <c r="I27" s="124"/>
-      <c r="J27" s="124"/>
-      <c r="K27" s="124"/>
-      <c r="L27" s="123"/>
-      <c r="M27" s="125"/>
-      <c r="N27" s="123"/>
-      <c r="O27" s="123"/>
-      <c r="P27" s="123"/>
-      <c r="Q27" s="124"/>
-      <c r="R27" s="126"/>
+      <c r="E27" s="114"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="116"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="116"/>
+      <c r="M27" s="118"/>
+      <c r="N27" s="116"/>
+      <c r="O27" s="116"/>
+      <c r="P27" s="116"/>
+      <c r="Q27" s="117"/>
+      <c r="R27" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>